<commit_message>
one change made on model and ER
</commit_message>
<xml_diff>
--- a/Software EVISA version Johan/Modelos/Modelo Relacional Excel.xlsx
+++ b/Software EVISA version Johan/Modelos/Modelo Relacional Excel.xlsx
@@ -287,10 +287,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13:S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,11 +643,11 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
@@ -727,9 +727,6 @@
       <c r="O5" t="s">
         <v>44</v>
       </c>
-      <c r="P5" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -777,9 +774,6 @@
       <c r="O6" t="s">
         <v>9</v>
       </c>
-      <c r="P6" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -858,6 +852,9 @@
       <c r="R13" t="s">
         <v>58</v>
       </c>
+      <c r="S13" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -914,6 +911,9 @@
       <c r="R14" t="s">
         <v>7</v>
       </c>
+      <c r="S14" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -922,10 +922,10 @@
       <c r="B15" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -988,11 +988,11 @@
       <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -1049,11 +1049,11 @@
       <c r="B31" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
@@ -1103,10 +1103,10 @@
       <c r="B40" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="4"/>
+      <c r="D40" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
@@ -1156,10 +1156,10 @@
       <c r="B50" t="s">
         <v>23</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D50" s="4"/>
+      <c r="D50" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
se agregaron los script para crear la BD .sql
</commit_message>
<xml_diff>
--- a/Software EVISA version Johan/Modelos/Modelo Relacional Excel.xlsx
+++ b/Software EVISA version Johan/Modelos/Modelo Relacional Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="85">
   <si>
     <t>id</t>
   </si>
@@ -253,6 +253,27 @@
   </si>
   <si>
     <t>"Requerimientos"</t>
+  </si>
+  <si>
+    <t>Meaning</t>
+  </si>
+  <si>
+    <t>tamizaje</t>
+  </si>
+  <si>
+    <t>espacio en grupo</t>
+  </si>
+  <si>
+    <t>unique, not_null</t>
+  </si>
+  <si>
+    <t>not_null</t>
+  </si>
+  <si>
+    <t>not_null, default(costa rica)</t>
+  </si>
+  <si>
+    <t>La tabla people_datasets se refiere a las personas que deben ser referidas al hospital no a la relación 1:N entre ellas la cual se refiere a los datos de esa persona.</t>
   </si>
 </sst>
 </file>
@@ -323,6 +344,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -330,14 +359,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -620,17 +641,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V61"/>
+  <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" customWidth="1"/>
     <col min="6" max="6" width="10.140625" customWidth="1"/>
     <col min="9" max="9" width="10.28515625" customWidth="1"/>
@@ -639,80 +660,82 @@
     <col min="13" max="13" width="11" customWidth="1"/>
     <col min="14" max="14" width="11.140625" customWidth="1"/>
     <col min="15" max="15" width="10.28515625" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
     </row>
     <row r="2" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="4" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
@@ -821,531 +844,645 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="N12" t="s">
-        <v>13</v>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" t="s">
-        <v>47</v>
-      </c>
-      <c r="H13" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13" t="s">
-        <v>49</v>
-      </c>
-      <c r="J13" t="s">
-        <v>50</v>
-      </c>
-      <c r="K13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M13" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="N13" t="s">
-        <v>54</v>
-      </c>
-      <c r="O13" t="s">
-        <v>55</v>
-      </c>
-      <c r="P13" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>57</v>
-      </c>
-      <c r="R13" t="s">
-        <v>58</v>
-      </c>
-      <c r="S13" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="G14" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="H14" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="I14" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="J14" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="K14" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="L14" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="M14" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="N14" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="O14" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="P14" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="Q14" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="R14" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="S14" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15" t="s">
+        <v>10</v>
+      </c>
+      <c r="P15" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>8</v>
+      </c>
+      <c r="R15" t="s">
+        <v>7</v>
+      </c>
+      <c r="S15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C17" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21" t="s">
-        <v>60</v>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B26" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C26" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" t="s">
-        <v>62</v>
-      </c>
-      <c r="E29" t="s">
-        <v>63</v>
-      </c>
-      <c r="F29" t="s">
-        <v>64</v>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B34" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D34" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35" t="s">
+        <v>82</v>
+      </c>
+      <c r="F35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B40" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B41" t="s">
         <v>0</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C41" t="s">
         <v>15</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D41" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B42" t="s">
         <v>11</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C42" t="s">
         <v>16</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D42" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B44" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C44" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+      <c r="D44" s="7"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B51" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B52" t="s">
         <v>0</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C52" t="s">
         <v>69</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D52" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B53" t="s">
         <v>11</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C53" t="s">
         <v>68</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D53" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B55" t="s">
         <v>23</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C55" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D54" s="9" t="s">
+      <c r="D55" s="7"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>82</v>
+      </c>
+      <c r="D56" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D59" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
-      <c r="K54" s="9"/>
-      <c r="L54" s="9"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D55" s="6">
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D60" s="3">
         <v>1</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="E60" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="7"/>
-      <c r="I55" s="7"/>
-      <c r="J55" s="7"/>
-      <c r="K55" s="7"/>
-      <c r="L55" s="7"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D56" s="6">
-        <f>D55+1</f>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="6"/>
+      <c r="K60" s="6"/>
+      <c r="L60" s="6"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D61" s="3">
+        <f>D60+1</f>
         <v>2</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="E61" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="7"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="7"/>
-      <c r="L56" s="7"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D57" s="6">
-        <f t="shared" ref="D57:D61" si="0">D56+1</f>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="6"/>
+      <c r="L61" s="6"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D62" s="3">
+        <f t="shared" ref="D62:D67" si="0">D61+1</f>
         <v>3</v>
       </c>
-      <c r="E57" s="7" t="s">
+      <c r="E62" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="7"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D58" s="6">
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="6"/>
+      <c r="L62" s="6"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D63" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E58" s="8" t="s">
+      <c r="E63" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
-      <c r="H58" s="8"/>
-      <c r="I58" s="8"/>
-      <c r="J58" s="8"/>
-      <c r="K58" s="8"/>
-      <c r="L58" s="8"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D59" s="6">
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="4"/>
+      <c r="L63" s="4"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D64" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E59" s="8" t="s">
+      <c r="E64" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
-      <c r="H59" s="8"/>
-      <c r="I59" s="8"/>
-      <c r="J59" s="8"/>
-      <c r="K59" s="8"/>
-      <c r="L59" s="8"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D60" s="6">
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+    </row>
+    <row r="65" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D65" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E60" s="8" t="s">
+      <c r="E65" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F60" s="8"/>
-      <c r="G60" s="8"/>
-      <c r="H60" s="8"/>
-      <c r="I60" s="8"/>
-      <c r="J60" s="8"/>
-      <c r="K60" s="8"/>
-      <c r="L60" s="8"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D61" s="6">
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="4"/>
+      <c r="L65" s="4"/>
+    </row>
+    <row r="66" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D66" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="E61" s="8" t="s">
+      <c r="E66" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F61" s="8"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="8"/>
-      <c r="I61" s="8"/>
-      <c r="J61" s="8"/>
-      <c r="K61" s="8"/>
-      <c r="L61" s="8"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="4"/>
+      <c r="L66" s="4"/>
+    </row>
+    <row r="67" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D67" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="E66:L66"/>
+    <mergeCell ref="E67:L67"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A1:S3"/>
+    <mergeCell ref="E65:L65"/>
+    <mergeCell ref="D59:L59"/>
     <mergeCell ref="E60:L60"/>
     <mergeCell ref="E61:L61"/>
-    <mergeCell ref="D54:L54"/>
-    <mergeCell ref="E55:L55"/>
-    <mergeCell ref="E56:L56"/>
-    <mergeCell ref="E57:L57"/>
-    <mergeCell ref="E58:L58"/>
-    <mergeCell ref="E59:L59"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A1:S3"/>
+    <mergeCell ref="E62:L62"/>
+    <mergeCell ref="E63:L63"/>
+    <mergeCell ref="E64:L64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
se corrigieron los modelos y se cargó al sitio web c9 de la bd
</commit_message>
<xml_diff>
--- a/Software EVISA version Johan/Modelos/Modelo Relacional Excel.xlsx
+++ b/Software EVISA version Johan/Modelos/Modelo Relacional Excel.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="106">
   <si>
     <t>id</t>
   </si>
@@ -69,9 +69,6 @@
     <t>location_id</t>
   </si>
   <si>
-    <t>location_id_fk</t>
-  </si>
-  <si>
     <t>person_id</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>group_id</t>
   </si>
   <si>
-    <t>group_id_fk</t>
-  </si>
-  <si>
     <t>autoincrement</t>
   </si>
   <si>
@@ -153,9 +147,6 @@
     <t>address</t>
   </si>
   <si>
-    <t>ebais</t>
-  </si>
-  <si>
     <t>social_security</t>
   </si>
   <si>
@@ -180,15 +171,9 @@
     <t>bmi</t>
   </si>
   <si>
-    <t>bmi_sort</t>
-  </si>
-  <si>
     <t>ia_score</t>
   </si>
   <si>
-    <t>sort</t>
-  </si>
-  <si>
     <t>screening_date</t>
   </si>
   <si>
@@ -204,9 +189,6 @@
     <t>space</t>
   </si>
   <si>
-    <t>country</t>
-  </si>
-  <si>
     <t>province</t>
   </si>
   <si>
@@ -252,9 +234,6 @@
     <t>Cada persona tiene una dirección, pero todos, tanto grupo como persona deben tener una localidad</t>
   </si>
   <si>
-    <t>"Requerimientos"</t>
-  </si>
-  <si>
     <t>Meaning</t>
   </si>
   <si>
@@ -274,12 +253,96 @@
   </si>
   <si>
     <t>La tabla people_datasets se refiere a las personas que deben ser referidas al hospital no a la relación 1:N entre ellas la cual se refiere a los datos de esa persona.</t>
+  </si>
+  <si>
+    <t>medical_center</t>
+  </si>
+  <si>
+    <t>sessions</t>
+  </si>
+  <si>
+    <t>goals</t>
+  </si>
+  <si>
+    <t>opening</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>feedfack</t>
+  </si>
+  <si>
+    <t>development</t>
+  </si>
+  <si>
+    <t>check_experience</t>
+  </si>
+  <si>
+    <t>varchar 50</t>
+  </si>
+  <si>
+    <t>date_time</t>
+  </si>
+  <si>
+    <t>intenger</t>
+  </si>
+  <si>
+    <t>duración en minutos</t>
+  </si>
+  <si>
+    <t>fecha y hora</t>
+  </si>
+  <si>
+    <t>Estas 4 variables son de tipo check e indican si se realizó o no por ej: definición de metas.</t>
+  </si>
+  <si>
+    <t>cédula</t>
+  </si>
+  <si>
+    <t>indice masa corp.</t>
+  </si>
+  <si>
+    <t>bmi_clasification</t>
+  </si>
+  <si>
+    <t>clasification</t>
+  </si>
+  <si>
+    <t>Riesgo o no riesgo</t>
+  </si>
+  <si>
+    <t>Entra o no al proceso de elección</t>
+  </si>
+  <si>
+    <t>people_sessions</t>
+  </si>
+  <si>
+    <t>session_id</t>
+  </si>
+  <si>
+    <t>sessions_id_fk</t>
+  </si>
+  <si>
+    <t>locations_id_fk</t>
+  </si>
+  <si>
+    <t>groups_id_fk</t>
+  </si>
+  <si>
+    <t>Recordatorio: para las relaciones 1:N identificadoras, dado que cake necesita el parámetro id por convención. Se define la llave foránea como NOT NULL</t>
+  </si>
+  <si>
+    <t>"Requerimientos" y restricciones</t>
+  </si>
+  <si>
+    <t>Muchas de las implementaciones se realizan de la forma que están por motivos de convenciones establecidas por el framework.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -340,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -348,10 +411,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -361,6 +420,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,117 +711,123 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="C82" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97:L97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" customWidth="1"/>
-    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.140625" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
+      <c r="A1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
     </row>
     <row r="2" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -759,51 +836,55 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>34</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>35</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>36</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>37</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" t="s">
         <v>38</v>
       </c>
-      <c r="J5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" t="s">
         <v>41</v>
       </c>
-      <c r="L5" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" t="s">
-        <v>42</v>
-      </c>
-      <c r="N5" t="s">
-        <v>43</v>
-      </c>
       <c r="O5" t="s">
-        <v>44</v>
+        <v>78</v>
+      </c>
+      <c r="P5">
+        <f>COUNTA(B5:O5)</f>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -844,38 +925,41 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
+      </c>
+      <c r="D7" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G8" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H8" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N13" t="s">
         <v>13</v>
@@ -883,58 +967,58 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" t="s">
         <v>45</v>
       </c>
-      <c r="F14" t="s">
+      <c r="I14" t="s">
         <v>46</v>
       </c>
-      <c r="G14" t="s">
+      <c r="J14" t="s">
         <v>47</v>
       </c>
-      <c r="H14" t="s">
+      <c r="K14" t="s">
         <v>48</v>
       </c>
-      <c r="I14" t="s">
+      <c r="L14" t="s">
         <v>49</v>
       </c>
-      <c r="J14" t="s">
+      <c r="M14" t="s">
+        <v>94</v>
+      </c>
+      <c r="N14" t="s">
         <v>50</v>
       </c>
-      <c r="K14" t="s">
+      <c r="O14" t="s">
+        <v>95</v>
+      </c>
+      <c r="P14" t="s">
         <v>51</v>
       </c>
-      <c r="L14" t="s">
+      <c r="Q14" t="s">
         <v>52</v>
       </c>
-      <c r="M14" t="s">
+      <c r="R14" t="s">
         <v>53</v>
-      </c>
-      <c r="N14" t="s">
-        <v>54</v>
-      </c>
-      <c r="O14" t="s">
-        <v>55</v>
-      </c>
-      <c r="P14" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>57</v>
-      </c>
-      <c r="R14" t="s">
-        <v>58</v>
       </c>
       <c r="S14" t="s">
         <v>1</v>
@@ -942,13 +1026,13 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
         <v>3</v>
@@ -1001,43 +1085,52 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J16" t="s">
-        <v>79</v>
+        <v>72</v>
+      </c>
+      <c r="L16" t="s">
+        <v>93</v>
+      </c>
+      <c r="O16" t="s">
+        <v>96</v>
+      </c>
+      <c r="S16" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
@@ -1046,27 +1139,27 @@
         <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F23" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G23" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
@@ -1083,67 +1176,64 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G25" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E27" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
         <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E31" t="s">
-        <v>63</v>
-      </c>
-      <c r="F31" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
@@ -1157,332 +1247,609 @@
       <c r="E32" t="s">
         <v>9</v>
       </c>
-      <c r="F32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
-      </c>
-      <c r="D34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D35" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E35" t="s">
-        <v>82</v>
-      </c>
-      <c r="F35" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B41" t="s">
         <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="E41" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" t="s">
+        <v>83</v>
+      </c>
+      <c r="G41" t="s">
+        <v>84</v>
+      </c>
+      <c r="H41" t="s">
+        <v>85</v>
+      </c>
+      <c r="I41" t="s">
+        <v>41</v>
+      </c>
+      <c r="J41" t="s">
+        <v>87</v>
+      </c>
+      <c r="K41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
       </c>
       <c r="C42" t="s">
+        <v>102</v>
+      </c>
+      <c r="D42" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" t="s">
+        <v>4</v>
+      </c>
+      <c r="H42" t="s">
+        <v>4</v>
+      </c>
+      <c r="I42" t="s">
+        <v>86</v>
+      </c>
+      <c r="J42" t="s">
+        <v>14</v>
+      </c>
+      <c r="K42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J43" t="s">
+        <v>90</v>
+      </c>
+      <c r="K43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="J44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>99</v>
+      </c>
+      <c r="D50" t="s">
         <v>16</v>
       </c>
-      <c r="D42" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B44" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D44" s="7"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>82</v>
-      </c>
-      <c r="D45" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B51" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C51" t="s">
+        <v>100</v>
+      </c>
+      <c r="D51" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="5"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>75</v>
+      </c>
+      <c r="D54" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B59" t="s">
         <v>0</v>
       </c>
-      <c r="C52" t="s">
-        <v>69</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="C59" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" t="s">
+        <v>101</v>
+      </c>
+      <c r="D60" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B62" t="s">
+        <v>21</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62" s="5"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>75</v>
+      </c>
+      <c r="D63" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B69" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B70" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>63</v>
+      </c>
+      <c r="D70" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B71" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71" t="s">
+        <v>62</v>
+      </c>
+      <c r="D71" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B53" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" t="s">
-        <v>68</v>
-      </c>
-      <c r="D53" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B55" t="s">
-        <v>23</v>
-      </c>
-      <c r="C55" s="7" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B73" t="s">
+        <v>21</v>
+      </c>
+      <c r="C73" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D55" s="7"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
-        <v>82</v>
-      </c>
-      <c r="D56" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D59" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
-      <c r="I59" s="5"/>
-      <c r="J59" s="5"/>
-      <c r="K59" s="5"/>
-      <c r="L59" s="5"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D60" s="3">
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>75</v>
+      </c>
+      <c r="D74" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="86" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D86" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E86" s="8"/>
+      <c r="F86" s="8"/>
+      <c r="G86" s="8"/>
+      <c r="H86" s="8"/>
+      <c r="I86" s="8"/>
+      <c r="J86" s="8"/>
+      <c r="K86" s="8"/>
+      <c r="L86" s="8"/>
+    </row>
+    <row r="87" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D87" s="3">
         <v>1</v>
       </c>
-      <c r="E60" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F60" s="6"/>
-      <c r="G60" s="6"/>
-      <c r="H60" s="6"/>
-      <c r="I60" s="6"/>
-      <c r="J60" s="6"/>
-      <c r="K60" s="6"/>
-      <c r="L60" s="6"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D61" s="3">
-        <f>D60+1</f>
+      <c r="E87" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+      <c r="H87" s="9"/>
+      <c r="I87" s="9"/>
+      <c r="J87" s="9"/>
+      <c r="K87" s="9"/>
+      <c r="L87" s="9"/>
+    </row>
+    <row r="88" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D88" s="3">
+        <f>D87+1</f>
         <v>2</v>
       </c>
-      <c r="E61" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F61" s="6"/>
-      <c r="G61" s="6"/>
-      <c r="H61" s="6"/>
-      <c r="I61" s="6"/>
-      <c r="J61" s="6"/>
-      <c r="K61" s="6"/>
-      <c r="L61" s="6"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D62" s="3">
-        <f t="shared" ref="D62:D67" si="0">D61+1</f>
+      <c r="E88" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F88" s="9"/>
+      <c r="G88" s="9"/>
+      <c r="H88" s="9"/>
+      <c r="I88" s="9"/>
+      <c r="J88" s="9"/>
+      <c r="K88" s="9"/>
+      <c r="L88" s="9"/>
+    </row>
+    <row r="89" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D89" s="3">
+        <f t="shared" ref="D89:D94" si="0">D88+1</f>
         <v>3</v>
       </c>
-      <c r="E62" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F62" s="6"/>
-      <c r="G62" s="6"/>
-      <c r="H62" s="6"/>
-      <c r="I62" s="6"/>
-      <c r="J62" s="6"/>
-      <c r="K62" s="6"/>
-      <c r="L62" s="6"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D63" s="3">
+      <c r="E89" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F89" s="9"/>
+      <c r="G89" s="9"/>
+      <c r="H89" s="9"/>
+      <c r="I89" s="9"/>
+      <c r="J89" s="9"/>
+      <c r="K89" s="9"/>
+      <c r="L89" s="9"/>
+    </row>
+    <row r="90" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D90" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E63" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D64" s="3">
+      <c r="E90" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
+      <c r="L90" s="4"/>
+    </row>
+    <row r="91" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D91" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E64" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-    </row>
-    <row r="65" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D65" s="3">
+      <c r="E91" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="4"/>
+      <c r="J91" s="4"/>
+      <c r="K91" s="4"/>
+      <c r="L91" s="4"/>
+    </row>
+    <row r="92" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D92" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E65" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="4"/>
-    </row>
-    <row r="66" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D66" s="3">
+      <c r="E92" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="4"/>
+      <c r="J92" s="4"/>
+      <c r="K92" s="4"/>
+      <c r="L92" s="4"/>
+    </row>
+    <row r="93" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D93" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="E66" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F66" s="4"/>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
-    </row>
-    <row r="67" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D67" s="3">
+      <c r="E93" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
+      <c r="J93" s="4"/>
+      <c r="K93" s="4"/>
+      <c r="L93" s="4"/>
+    </row>
+    <row r="94" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D94" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E67" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="4"/>
-      <c r="J67" s="4"/>
-      <c r="K67" s="4"/>
-      <c r="L67" s="4"/>
+      <c r="E94" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F94" s="4"/>
+      <c r="G94" s="4"/>
+      <c r="H94" s="4"/>
+      <c r="I94" s="4"/>
+      <c r="J94" s="4"/>
+      <c r="K94" s="4"/>
+      <c r="L94" s="4"/>
+    </row>
+    <row r="95" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D95" s="11">
+        <v>9</v>
+      </c>
+      <c r="E95" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="F95" s="12"/>
+      <c r="G95" s="12"/>
+      <c r="H95" s="12"/>
+      <c r="I95" s="12"/>
+      <c r="J95" s="12"/>
+      <c r="K95" s="12"/>
+      <c r="L95" s="12"/>
+      <c r="M95" s="10"/>
+    </row>
+    <row r="96" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D96" s="11">
+        <v>10</v>
+      </c>
+      <c r="E96" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="F96" s="13"/>
+      <c r="G96" s="13"/>
+      <c r="H96" s="13"/>
+      <c r="I96" s="13"/>
+      <c r="J96" s="13"/>
+      <c r="K96" s="13"/>
+      <c r="L96" s="13"/>
+    </row>
+    <row r="97" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D97" s="11"/>
+      <c r="E97" s="13"/>
+      <c r="F97" s="13"/>
+      <c r="G97" s="13"/>
+      <c r="H97" s="13"/>
+      <c r="I97" s="13"/>
+      <c r="J97" s="13"/>
+      <c r="K97" s="13"/>
+      <c r="L97" s="13"/>
+    </row>
+    <row r="98" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D98" s="11"/>
+      <c r="E98" s="13"/>
+      <c r="F98" s="13"/>
+      <c r="G98" s="13"/>
+      <c r="H98" s="13"/>
+      <c r="I98" s="13"/>
+      <c r="J98" s="13"/>
+      <c r="K98" s="13"/>
+      <c r="L98" s="13"/>
+    </row>
+    <row r="99" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D99" s="11"/>
+      <c r="E99" s="13"/>
+      <c r="F99" s="13"/>
+      <c r="G99" s="13"/>
+      <c r="H99" s="13"/>
+      <c r="I99" s="13"/>
+      <c r="J99" s="13"/>
+      <c r="K99" s="13"/>
+      <c r="L99" s="13"/>
+    </row>
+    <row r="100" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D100" s="11"/>
+      <c r="E100" s="13"/>
+      <c r="F100" s="13"/>
+      <c r="G100" s="13"/>
+      <c r="H100" s="13"/>
+      <c r="I100" s="13"/>
+      <c r="J100" s="13"/>
+      <c r="K100" s="13"/>
+      <c r="L100" s="13"/>
+    </row>
+    <row r="101" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D101" s="11"/>
+      <c r="E101" s="13"/>
+      <c r="F101" s="13"/>
+      <c r="G101" s="13"/>
+      <c r="H101" s="13"/>
+      <c r="I101" s="13"/>
+      <c r="J101" s="13"/>
+      <c r="K101" s="13"/>
+      <c r="L101" s="13"/>
+    </row>
+    <row r="102" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D102" s="11"/>
+      <c r="E102" s="13"/>
+      <c r="F102" s="13"/>
+      <c r="G102" s="13"/>
+      <c r="H102" s="13"/>
+      <c r="I102" s="13"/>
+      <c r="J102" s="13"/>
+      <c r="K102" s="13"/>
+      <c r="L102" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="E66:L66"/>
-    <mergeCell ref="E67:L67"/>
-    <mergeCell ref="C55:D55"/>
+  <mergeCells count="26">
+    <mergeCell ref="E102:L102"/>
+    <mergeCell ref="E97:L97"/>
+    <mergeCell ref="E98:L98"/>
+    <mergeCell ref="E99:L99"/>
+    <mergeCell ref="E100:L100"/>
+    <mergeCell ref="E101:L101"/>
+    <mergeCell ref="D44:H44"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E95:L95"/>
+    <mergeCell ref="E96:L96"/>
+    <mergeCell ref="E93:L93"/>
+    <mergeCell ref="E94:L94"/>
+    <mergeCell ref="C73:D73"/>
     <mergeCell ref="T2:V2"/>
-    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C62:D62"/>
     <mergeCell ref="D34:F34"/>
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="A1:S3"/>
-    <mergeCell ref="E65:L65"/>
-    <mergeCell ref="D59:L59"/>
-    <mergeCell ref="E60:L60"/>
-    <mergeCell ref="E61:L61"/>
-    <mergeCell ref="E62:L62"/>
-    <mergeCell ref="E63:L63"/>
-    <mergeCell ref="E64:L64"/>
+    <mergeCell ref="E92:L92"/>
+    <mergeCell ref="D86:L86"/>
+    <mergeCell ref="E87:L87"/>
+    <mergeCell ref="E88:L88"/>
+    <mergeCell ref="E89:L89"/>
+    <mergeCell ref="E90:L90"/>
+    <mergeCell ref="E91:L91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>